<commit_message>
Actualizando a la DB
</commit_message>
<xml_diff>
--- a/Traduccion/excels/Core/Trad PHB.xlsx
+++ b/Traduccion/excels/Core/Trad PHB.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rol\Roll20\Repos github\5etoolsEsp\excels\Core\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programacion\JAVA\Proyectos\5etoolsEsp\Traduccion\excels\Core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A383EEE-954F-4C5A-A484-2E2FC795E2E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1D3530-E12E-4D29-AE0A-89D7D5045E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="854" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="854" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Indice" sheetId="1" r:id="rId1"/>
@@ -16850,7 +16850,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="B1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -17729,8 +17729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:D65"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18277,8 +18277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:D197"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B196" sqref="B196"/>
+    <sheetView topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="B197" sqref="B197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19931,8 +19931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Traducción de más objetos
</commit_message>
<xml_diff>
--- a/Traduccion/excels/Core/Trad PHB.xlsx
+++ b/Traduccion/excels/Core/Trad PHB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programacion\JAVA\Proyectos\5etoolsEsp\Traduccion\excels\Core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73720D1C-8D05-4309-B915-01C5F81D6F29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC7B731-1DB0-42AE-BF8E-F07C0445F810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="854" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="854" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Indice" sheetId="1" r:id="rId1"/>
@@ -9947,7 +9947,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="B1:D362"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A340" workbookViewId="0">
+    <sheetView topLeftCell="A340" workbookViewId="0">
       <selection activeCell="B362" sqref="B362"/>
     </sheetView>
   </sheetViews>
@@ -9969,7 +9969,7 @@
       </c>
       <c r="D1" s="5"/>
     </row>
-    <row r="2" spans="2:4" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>807</v>
       </c>
@@ -10041,7 +10041,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>825</v>
       </c>
@@ -10057,7 +10057,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>829</v>
       </c>
@@ -10153,7 +10153,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="25" spans="2:3" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>853</v>
       </c>
@@ -19877,8 +19877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>